<commit_message>
Adicionado tabela HTML no Emal. V.1.0.8
</commit_message>
<xml_diff>
--- a/Data/Input/Dados.xlsx
+++ b/Data/Input/Dados.xlsx
@@ -88,7 +88,7 @@
     <x:t>Econômica</x:t>
   </x:si>
   <x:si>
-    <x:t>R$ 3.186</x:t>
+    <x:t>R$ 3.173</x:t>
   </x:si>
   <x:si>
     <x:t>11/01/2023</x:t>
@@ -100,13 +100,13 @@
     <x:t>Lisboa, Portugal – Portela de Sacavém</x:t>
   </x:si>
   <x:si>
-    <x:t>R$ 2.803</x:t>
+    <x:t>R$ 2.626</x:t>
   </x:si>
   <x:si>
     <x:t>New York, USA – John F Kennedy Intl</x:t>
   </x:si>
   <x:si>
-    <x:t>R$ 3.184</x:t>
+    <x:t>R$ 3.093</x:t>
   </x:si>
   <x:si>
     <x:t>Rome, Italy – Leonardo Da Vinci / Fiumicino</x:t>

</xml_diff>